<commit_message>
added costs an extra insulation
</commit_message>
<xml_diff>
--- a/F-Heat_QGIS/data/pipe_data.xlsx
+++ b/F-Heat_QGIS/data/pipe_data.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lars_Goray\AppData\Roaming\QGIS\QGIS3\profiles\default\python\plugins\heat_net_tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA92BBE-5ED2-4332-A396-E9C6E3135B97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381E6D1A-8910-4FDC-9A1F-C153254B2656}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8508" xr2:uid="{AC4DDAF7-09D1-46D9-9EBE-54012C8EDE68}"/>
   </bookViews>
   <sheets>
     <sheet name="pipe_data" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>DN</t>
   </si>
@@ -52,6 +55,9 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>U-Value_extra_insulation</t>
   </si>
 </sst>
 </file>
@@ -168,6 +174,101 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Rehau Uno"/>
+      <sheetName val="FibreFLEX single"/>
+      <sheetName val="FibreFLEX PRO single"/>
+      <sheetName val="Rehau Duo"/>
+      <sheetName val="FibreFLEX double"/>
+      <sheetName val="FibreFLEX PRO double"/>
+      <sheetName val="Mittelwert Single"/>
+      <sheetName val="Mittelwert Double"/>
+      <sheetName val="ISOPLUS DRD"/>
+      <sheetName val="ISOPLUS KRE einzel"/>
+      <sheetName val="Logstor Twin Pipes"/>
+      <sheetName val="Rohre für Rechnung"/>
+      <sheetName val="Rohrverteilung nach Victor"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="14">
+          <cell r="J14">
+            <v>0.16200000000000001</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="J16">
+            <v>0.218</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3">
+        <row r="3">
+          <cell r="J3">
+            <v>0.129</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="J5">
+            <v>0.14299999999999999</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="J7">
+            <v>0.159</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="J9">
+            <v>0.151</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="J11">
+            <v>0.17799999999999999</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="J12">
+            <v>0.24299999999999999</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9">
+        <row r="9">
+          <cell r="G9">
+            <v>0.2228</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="G10">
+            <v>0.25340000000000001</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="G11">
+            <v>0.26769999999999999</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -467,21 +568,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF363AC-5F36-48EC-B9C0-91D761D69038}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" customWidth="1"/>
-    <col min="7" max="7" width="27.77734375" customWidth="1"/>
+    <col min="5" max="5" width="22.88671875" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" customWidth="1"/>
+    <col min="8" max="8" width="27.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
@@ -494,14 +596,17 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -515,13 +620,17 @@
         <v>0.129</v>
       </c>
       <c r="E2">
+        <f>'[1]Rehau Duo'!J3</f>
+        <v>0.129</v>
+      </c>
+      <c r="F2">
         <v>0.6</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.19611077980768923</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -535,13 +644,17 @@
         <v>0.16900000000000001</v>
       </c>
       <c r="E3">
+        <f>'[1]Rehau Duo'!J5</f>
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.53912871528254436</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -555,13 +668,17 @@
         <v>0.191</v>
       </c>
       <c r="E4">
+        <f>'[1]Rehau Duo'!J7</f>
+        <v>0.159</v>
+      </c>
+      <c r="F4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.91815872734549941</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -575,13 +692,17 @@
         <v>0.17799999999999999</v>
       </c>
       <c r="E5">
+        <f>'[1]Rehau Duo'!J9</f>
+        <v>0.151</v>
+      </c>
+      <c r="F5">
         <v>1.2</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>1.5688862384615139</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -595,13 +716,17 @@
         <v>0.21299999999999999</v>
       </c>
       <c r="E6">
+        <f>'[1]Rehau Duo'!J11</f>
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="F6">
         <v>1.4</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>2.9049867444773314</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -615,13 +740,17 @@
         <v>0.24299999999999999</v>
       </c>
       <c r="E7">
+        <f>'[1]Rehau Duo'!J12</f>
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="F7">
         <v>1.6</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>4.737471456130951</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -635,13 +764,17 @@
         <v>0.19</v>
       </c>
       <c r="E8">
+        <f>'[1]Rehau Uno'!J14</f>
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="F8">
         <v>1.8</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>7.6580467833553927</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -655,13 +788,17 @@
         <v>0.27400000000000002</v>
       </c>
       <c r="E9">
+        <f>'[1]Rehau Uno'!J16</f>
+        <v>0.218</v>
+      </c>
+      <c r="F9">
         <v>1.9</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>12.08727773468673</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -675,13 +812,17 @@
         <v>0.26200000000000001</v>
       </c>
       <c r="E10">
+        <f>'[1]ISOPLUS KRE einzel'!G9</f>
+        <v>0.2228</v>
+      </c>
+      <c r="F10">
         <v>1.8</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>24.819563711063612</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -695,13 +836,17 @@
         <v>0.30740000000000001</v>
       </c>
       <c r="E11">
+        <f>'[1]ISOPLUS KRE einzel'!G10</f>
+        <v>0.25340000000000001</v>
+      </c>
+      <c r="F11">
         <v>2.1</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>42.381489974240637</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -715,13 +860,17 @@
         <v>0.33610000000000001</v>
       </c>
       <c r="E12">
+        <f>'[1]ISOPLUS KRE einzel'!G11</f>
+        <v>0.26769999999999999</v>
+      </c>
+      <c r="F12">
         <v>2.4</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>83.205728598412293</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -735,13 +884,16 @@
         <v>0.38229999999999997</v>
       </c>
       <c r="E13">
+        <v>0.29830000000000001</v>
+      </c>
+      <c r="F13">
         <v>2.7</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>146.67805502290287</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -755,9 +907,12 @@
         <v>0.44169999999999998</v>
       </c>
       <c r="E14">
+        <v>0.34129999999999999</v>
+      </c>
+      <c r="F14">
         <v>3</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>230.39173674189982</v>
       </c>
     </row>

</xml_diff>